<commit_message>
added changes to the width
added changes to the width
</commit_message>
<xml_diff>
--- a/LE4/Uber_Kartenanwendung_Evaluationsprotokoll_Enhanced.xlsx
+++ b/LE4/Uber_Kartenanwendung_Evaluationsprotokoll_Enhanced.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\super\Documents\GitHub\IVI\FHNW_IVI_2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\super\Documents\GitHub\IVI\FHNW_IVI_2023\LE4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6DFC861D-D996-4CC4-B3B2-AB94AA76F42E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5159F24F-ACAA-4BD0-A9A7-18340FE6500D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="77040" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="61350" yWindow="90" windowWidth="15450" windowHeight="21525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Evaluation" sheetId="1" r:id="rId1"/>
@@ -59,9 +59,6 @@
     <t>Anpassungsfähigkeit</t>
   </si>
   <si>
-    <t>Bewertung 1 - Person J.S</t>
-  </si>
-  <si>
     <t>Bewertung 2 Person A.M</t>
   </si>
   <si>
@@ -168,6 +165,9 @@
   </si>
   <si>
     <t>Kriterien:</t>
+  </si>
+  <si>
+    <t>Bewertung 1 - Person N.R</t>
   </si>
 </sst>
 </file>
@@ -325,28 +325,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -355,6 +349,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -663,15 +660,15 @@
   <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="5" width="12.7109375" customWidth="1"/>
-    <col min="6" max="6" width="85.28515625" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
     <col min="7" max="7" width="20.7109375" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" customWidth="1"/>
   </cols>
@@ -681,23 +678,23 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2">
@@ -712,533 +709,540 @@
       <c r="E2" s="2">
         <v>4</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="4">
         <f>AVERAGE(B2:E2)</f>
         <v>4.25</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="7">
-        <v>2</v>
-      </c>
-      <c r="C3" s="7">
+      <c r="B3">
         <v>3</v>
       </c>
-      <c r="D3" s="7">
-        <v>5</v>
-      </c>
-      <c r="E3" s="12">
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
         <v>4</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="6">
         <f t="shared" ref="F3:F7" si="0">AVERAGE(B3:E3)</f>
-        <v>3.5</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="7">
-        <v>5</v>
-      </c>
-      <c r="C4" s="7">
-        <v>5</v>
-      </c>
-      <c r="D4" s="7">
-        <v>5</v>
-      </c>
-      <c r="E4" s="12">
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
         <v>4</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="6">
         <f t="shared" si="0"/>
         <v>4.75</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="7">
-        <v>5</v>
-      </c>
-      <c r="C5" s="7">
-        <v>5</v>
-      </c>
-      <c r="D5" s="7">
-        <v>5</v>
-      </c>
-      <c r="E5" s="12">
+      <c r="A5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
         <v>4</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="6">
         <f t="shared" si="0"/>
         <v>4.75</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="7">
-        <v>5</v>
-      </c>
-      <c r="C6" s="7">
-        <v>5</v>
-      </c>
-      <c r="D6" s="7">
-        <v>5</v>
-      </c>
-      <c r="E6" s="12">
-        <v>5</v>
-      </c>
-      <c r="F6" s="8">
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="10">
-        <v>5</v>
-      </c>
-      <c r="C7" s="10">
-        <v>5</v>
-      </c>
-      <c r="D7" s="10">
+      <c r="B7" s="8">
+        <v>5</v>
+      </c>
+      <c r="C7" s="8">
+        <v>5</v>
+      </c>
+      <c r="D7" s="8">
         <v>4</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="8">
         <v>4</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="9">
         <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F8" s="14">
+      <c r="F8" s="6">
         <f>AVERAGE(F2:F7)</f>
-        <v>4.458333333333333</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
+      <c r="C13" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="C16" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B19" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B20" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
+      <c r="C20" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
+      <c r="C23" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B26" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
+      <c r="C26" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B27" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
+      <c r="C28" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>6</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
+      <c r="C30" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
+      <c r="C31" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B33" t="s">
         <v>2</v>
       </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B34" t="s">
         <v>3</v>
       </c>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>4</v>
       </c>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>6</v>
       </c>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>7</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
+      <c r="C38" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="16" t="s">
+      <c r="A45" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="11"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="11"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="15"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="15"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="17" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="17" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="11"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="15"/>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="16" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="11"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="11"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="15"/>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="15"/>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="17" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="13" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="17" t="s">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="11"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="15"/>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="16" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="11"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="11"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="13" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="15"/>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="15"/>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="17" t="s">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="17" t="s">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="11"/>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="15"/>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="16" t="s">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="11"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="11"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="15"/>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="15"/>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="17" t="s">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="17" t="s">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="11"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="12" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="15"/>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="16" t="s">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="11"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="11"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="15"/>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="15"/>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="17" t="s">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="13" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="17" t="s">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="11"/>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="12" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="15"/>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="16" t="s">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="11"/>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="11"/>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="13" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="15"/>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="15"/>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" s="17" t="s">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="13" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="17" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="C34:F34"/>
-    <mergeCell ref="C35:F35"/>
-    <mergeCell ref="C36:F36"/>
-    <mergeCell ref="C37:F37"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C23:F23"/>
     <mergeCell ref="C38:F38"/>
     <mergeCell ref="C26:F26"/>
     <mergeCell ref="C27:F27"/>
@@ -1246,18 +1250,11 @@
     <mergeCell ref="C29:F29"/>
     <mergeCell ref="C30:F30"/>
     <mergeCell ref="C31:F31"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="C34:F34"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="C36:F36"/>
+    <mergeCell ref="C37:F37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1265,6 +1262,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="7f1f0d97-ec5c-498e-b12e-f18a1b1e791d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F20B0873802AEC438A03CD3AC20D0FCD" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cea4b96a48bcca927c0a048bfdb2d8f9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="7f1f0d97-ec5c-498e-b12e-f18a1b1e791d" xmlns:ns4="c9e1ce74-352a-4e51-b14f-5ea2d90be007" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1e54fe38165d9390254e60811d504efb" ns3:_="" ns4:_="">
     <xsd:import namespace="7f1f0d97-ec5c-498e-b12e-f18a1b1e791d"/>
@@ -1505,24 +1519,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5715F34-7FB1-4F63-9510-256B1ED587B7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="7f1f0d97-ec5c-498e-b12e-f18a1b1e791d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="c9e1ce74-352a-4e51-b14f-5ea2d90be007"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="7f1f0d97-ec5c-498e-b12e-f18a1b1e791d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00310CD1-D4CE-4223-AAD2-B128ECC51AD0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE24767-0CB7-494B-84DF-3BB0608FDF1F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1539,29 +1561,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00310CD1-D4CE-4223-AAD2-B128ECC51AD0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5715F34-7FB1-4F63-9510-256B1ED587B7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="7f1f0d97-ec5c-498e-b12e-f18a1b1e791d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="c9e1ce74-352a-4e51-b14f-5ea2d90be007"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
change name final and excel modifyed
change name final and excel modifyed
</commit_message>
<xml_diff>
--- a/LE4/Uber_Kartenanwendung_Evaluationsprotokoll_Enhanced.xlsx
+++ b/LE4/Uber_Kartenanwendung_Evaluationsprotokoll_Enhanced.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\super\Documents\GitHub\IVI\FHNW_IVI_2023\LE4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5159F24F-ACAA-4BD0-A9A7-18340FE6500D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD2900A4-AA52-4787-9F5D-6C0F9612A5F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="61350" yWindow="90" windowWidth="15450" windowHeight="21525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="46">
   <si>
     <t>Kriterium</t>
   </si>
@@ -68,9 +68,6 @@
     <t>Bemerkungen:</t>
   </si>
   <si>
-    <t>J.S</t>
-  </si>
-  <si>
     <t>A.M</t>
   </si>
   <si>
@@ -168,6 +165,12 @@
   </si>
   <si>
     <t>Bewertung 1 - Person N.R</t>
+  </si>
+  <si>
+    <t>N.R</t>
+  </si>
+  <si>
+    <t>Was zeigen eigentlich die grösse der Punkte an?</t>
   </si>
 </sst>
 </file>
@@ -660,7 +663,7 @@
   <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,7 +681,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>8</v>
@@ -687,7 +690,7 @@
         <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>1</v>
@@ -839,13 +842,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
@@ -864,7 +867,9 @@
       <c r="B15" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="14"/>
+      <c r="C15" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
@@ -874,7 +879,7 @@
         <v>6</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D16" s="14"/>
       <c r="E16" s="14"/>
@@ -903,13 +908,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B20" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
@@ -938,7 +943,7 @@
         <v>6</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
@@ -961,7 +966,7 @@
         <v>2</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
@@ -969,7 +974,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B27" t="s">
         <v>3</v>
@@ -984,7 +989,7 @@
         <v>4</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
@@ -1004,7 +1009,7 @@
         <v>6</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D30" s="14"/>
       <c r="E30" s="14"/>
@@ -1015,7 +1020,7 @@
         <v>7</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D31" s="14"/>
       <c r="E31" s="14"/>
@@ -1035,7 +1040,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B34" t="s">
         <v>3</v>
@@ -1077,7 +1082,7 @@
         <v>7</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D38" s="14"/>
       <c r="E38" s="14"/>
@@ -1085,12 +1090,12 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1101,12 +1106,12 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
@@ -1114,7 +1119,7 @@
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
@@ -1125,12 +1130,12 @@
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
@@ -1138,7 +1143,7 @@
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
@@ -1149,12 +1154,12 @@
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
@@ -1162,7 +1167,7 @@
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
@@ -1173,12 +1178,12 @@
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
@@ -1186,7 +1191,7 @@
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
@@ -1197,12 +1202,12 @@
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
@@ -1210,7 +1215,7 @@
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
@@ -1221,16 +1226,28 @@
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="C38:F38"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="C34:F34"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="C36:F36"/>
+    <mergeCell ref="C37:F37"/>
     <mergeCell ref="C24:F24"/>
     <mergeCell ref="C12:F12"/>
     <mergeCell ref="C13:F13"/>
@@ -1243,18 +1260,6 @@
     <mergeCell ref="C21:F21"/>
     <mergeCell ref="C22:F22"/>
     <mergeCell ref="C23:F23"/>
-    <mergeCell ref="C38:F38"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="C34:F34"/>
-    <mergeCell ref="C35:F35"/>
-    <mergeCell ref="C36:F36"/>
-    <mergeCell ref="C37:F37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1262,23 +1267,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="7f1f0d97-ec5c-498e-b12e-f18a1b1e791d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F20B0873802AEC438A03CD3AC20D0FCD" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cea4b96a48bcca927c0a048bfdb2d8f9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="7f1f0d97-ec5c-498e-b12e-f18a1b1e791d" xmlns:ns4="c9e1ce74-352a-4e51-b14f-5ea2d90be007" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1e54fe38165d9390254e60811d504efb" ns3:_="" ns4:_="">
     <xsd:import namespace="7f1f0d97-ec5c-498e-b12e-f18a1b1e791d"/>
@@ -1519,32 +1507,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5715F34-7FB1-4F63-9510-256B1ED587B7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="7f1f0d97-ec5c-498e-b12e-f18a1b1e791d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="c9e1ce74-352a-4e51-b14f-5ea2d90be007"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00310CD1-D4CE-4223-AAD2-B128ECC51AD0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="7f1f0d97-ec5c-498e-b12e-f18a1b1e791d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE24767-0CB7-494B-84DF-3BB0608FDF1F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1561,4 +1541,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00310CD1-D4CE-4223-AAD2-B128ECC51AD0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5715F34-7FB1-4F63-9510-256B1ED587B7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="7f1f0d97-ec5c-498e-b12e-f18a1b1e791d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="c9e1ce74-352a-4e51-b14f-5ea2d90be007"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>